<commit_message>
fix crash + pm2
</commit_message>
<xml_diff>
--- a/modules/log/Kanat.xlsx
+++ b/modules/log/Kanat.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N14"/>
+  <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -1018,9 +1018,53 @@
         <v>10</v>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>Kanat</v>
+      </c>
+      <c r="B15" t="str">
+        <v>9913</v>
+      </c>
+      <c r="C15" t="str">
+        <v>Байсеркешов А</v>
+      </c>
+      <c r="D15" t="str">
+        <v>Толе би (Комешбулак)</v>
+      </c>
+      <c r="E15" t="str">
+        <v>21/1</v>
+      </c>
+      <c r="F15" t="str">
+        <v>10345</v>
+      </c>
+      <c r="G15" t="str">
+        <v>1860</v>
+      </c>
+      <c r="H15" t="str">
+        <v>1866</v>
+      </c>
+      <c r="I15" t="str">
+        <v>6</v>
+      </c>
+      <c r="J15" t="str">
+        <v>2025</v>
+      </c>
+      <c r="K15" t="str">
+        <v>5</v>
+      </c>
+      <c r="L15" t="str">
+        <v>22</v>
+      </c>
+      <c r="M15" t="str">
+        <v>20</v>
+      </c>
+      <c r="N15" t="str">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N14"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N15"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>